<commit_message>
HW Negative Login Test using DataProvider
</commit_message>
<xml_diff>
--- a/testData/ExelenterEmployeesList.xlsx
+++ b/testData/ExelenterEmployeesList.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnoza/IdeaProjects/TestNGProject/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA457C23-EB84-5040-81B3-5C88A74157F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AF7C86-990F-4541-B618-5A081E9FF625}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18020" yWindow="-16700" windowWidth="26040" windowHeight="13980" xr2:uid="{7A12BD58-98C9-E048-8107-5573E8AB6C07}"/>
+    <workbookView xWindow="-7640" yWindow="-16300" windowWidth="17800" windowHeight="13980" activeTab="2" xr2:uid="{7A12BD58-98C9-E048-8107-5573E8AB6C07}"/>
   </bookViews>
   <sheets>
     <sheet name="Employee" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="NegativeLoginTests" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="39">
   <si>
     <t>Firstname</t>
   </si>
@@ -83,23 +85,80 @@
     <t>johnSmith_@2023!!!</t>
   </si>
   <si>
-    <t>willadams12</t>
-  </si>
-  <si>
-    <t>elizabethlee12</t>
-  </si>
-  <si>
-    <t>tylernguyen12</t>
-  </si>
-  <si>
-    <t>johnSmith12</t>
+    <t>Acceptance Criteria:</t>
+  </si>
+  <si>
+    <t>invalid</t>
+  </si>
+  <si>
+    <t>Error Message</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>Invalid credentials</t>
+  </si>
+  <si>
+    <t>valid</t>
+  </si>
+  <si>
+    <t xml:space="preserve">invalid </t>
+  </si>
+  <si>
+    <t>empty</t>
+  </si>
+  <si>
+    <t>Password cannot be empty</t>
+  </si>
+  <si>
+    <t>Username cannot be empty</t>
+  </si>
+  <si>
+    <t>Negative Login Testing</t>
+  </si>
+  <si>
+    <t>User Story: US 12567: As an Invalid User, I should not be able to login using invalid login credentials, and when I try, I should see an error message.</t>
+  </si>
+  <si>
+    <t>willadams123</t>
+  </si>
+  <si>
+    <t>elizabethlee132</t>
+  </si>
+  <si>
+    <t>tylernguyen132</t>
+  </si>
+  <si>
+    <t>johnSmith132</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>errorMessage</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>invalidPass</t>
+  </si>
+  <si>
+    <t>admi123</t>
+  </si>
+  <si>
+    <t>Exelent2022Sdet!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -129,13 +188,48 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -151,10 +245,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -472,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57988F14-CEFA-C548-B8A8-EA00BB470A14}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -506,7 +622,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -520,7 +636,7 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
@@ -534,7 +650,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -548,7 +664,7 @@
         <v>14</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>15</v>
@@ -562,4 +678,293 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D2FA15-2832-3E44-980E-E0C5E162A2FE}">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="3"/>
+    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+    </row>
+    <row r="2" spans="1:6" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="5"/>
+    </row>
+    <row r="4" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G18" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC95BE32-01C2-FC48-87CD-8CA176A20787}">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9"/>
+      <c r="B7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="9"/>
+      <c r="B8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="9"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>